<commit_message>
Change test data for cta services
</commit_message>
<xml_diff>
--- a/Exceldata/CTASDDI.xlsx
+++ b/Exceldata/CTASDDI.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13215" windowHeight="2910" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13215" windowHeight="2910" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ModifyLegalClass" sheetId="3" r:id="rId1"/>
     <sheet name="ModifyTL" sheetId="9" r:id="rId2"/>
     <sheet name="ModifyChangeName" sheetId="10" r:id="rId3"/>
     <sheet name="cta_activities" sheetId="4" r:id="rId4"/>
-    <sheet name="ReviewTL" sheetId="8" r:id="rId5"/>
-    <sheet name="UpdateTL" sheetId="5" r:id="rId6"/>
-    <sheet name="ReviewTLAfterUpdate" sheetId="6" r:id="rId7"/>
+    <sheet name="NewNocForCounter" sheetId="11" r:id="rId5"/>
+    <sheet name="ReviewTL" sheetId="8" r:id="rId6"/>
+    <sheet name="UpdateTL" sheetId="5" r:id="rId7"/>
+    <sheet name="ReviewTLAfterUpdate" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">cta_activities!$A$1:$B$24</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
   <si>
     <t>Yes</t>
   </si>
@@ -171,13 +172,16 @@
   </si>
   <si>
     <t>Cat_ID</t>
+  </si>
+  <si>
+    <t>500.00 AED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,8 +230,23 @@
       <name val="Dubai"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Dubai"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,8 +277,20 @@
         <bgColor theme="8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor theme="8" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -278,12 +309,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -295,12 +421,21 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
       <font>
         <strike val="0"/>
@@ -308,81 +443,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Dubai"/>
-        <scheme val="none"/>
+        <sz val="10"/>
+        <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
           <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Dubai"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Dubai"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Dubai"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -427,6 +493,91 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Dubai"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Dubai"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Dubai"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Dubai"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -441,23 +592,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B10" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C8" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C8"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Cat_ID"/>
+    <tableColumn id="2" name="srvFee"/>
+    <tableColumn id="3" name="New Legal Class"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B10" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:B10"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Cat_ID" dataDxfId="3"/>
-    <tableColumn id="2" name="srvFee" dataDxfId="2"/>
+    <tableColumn id="1" name="Cat_ID" dataDxfId="7"/>
+    <tableColumn id="2" name="srvFee" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C24" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:C24"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Code" dataDxfId="8"/>
-    <tableColumn id="2" name="Obligation" dataDxfId="7" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="srvFee" dataDxfId="6"/>
+    <tableColumn id="1" name="Code" dataDxfId="3"/>
+    <tableColumn id="2" name="Obligation" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="srvFee" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -726,30 +889,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="19.5" x14ac:dyDescent="0.5">
+      <c r="A2" s="10">
+        <v>10081</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -793,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.5"/>
@@ -814,7 +993,7 @@
     </row>
     <row r="2" spans="1:2" ht="20.25" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A2" s="10">
-        <v>170</v>
+        <v>10081</v>
       </c>
       <c r="B2" s="10">
         <v>100</v>
@@ -834,7 +1013,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,6 +1291,47 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1146,7 +1366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1184,7 +1404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
- Change expected event count to be zero - Change ER db Name
</commit_message>
<xml_diff>
--- a/Exceldata/CTASDDI.xlsx
+++ b/Exceldata/CTASDDI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13215" windowHeight="2910" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13215" windowHeight="2910" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ModifyLegalClass" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="ReviewTLAfterUpdate" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">cta_activities!$A$1:$B$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">cta_activities!$A$1:$B$31</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="51">
   <si>
     <t>Yes</t>
   </si>
@@ -69,9 +69,6 @@
     <t>990076</t>
   </si>
   <si>
-    <t>161</t>
-  </si>
-  <si>
     <t>162</t>
   </si>
   <si>
@@ -175,13 +172,28 @@
   </si>
   <si>
     <t>500.00 AED</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>990075</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +257,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -409,7 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -430,28 +448,13 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -578,6 +581,22 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -592,7 +611,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C8" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C8" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:C8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Cat_ID"/>
@@ -604,23 +623,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B10" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:B10"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Cat_ID" dataDxfId="7"/>
-    <tableColumn id="2" name="srvFee" dataDxfId="6"/>
+    <tableColumn id="1" name="Cat_ID" dataDxfId="6"/>
+    <tableColumn id="2" name="srvFee" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C24" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:C24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C31" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C31"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Code" dataDxfId="3"/>
-    <tableColumn id="2" name="Obligation" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="srvFee" dataDxfId="1"/>
+    <tableColumn id="1" name="Code" dataDxfId="2"/>
+    <tableColumn id="2" name="Obligation" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="srvFee" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -903,10 +922,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>5</v>
@@ -917,7 +936,7 @@
         <v>10081</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -948,18 +967,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -985,10 +1004,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="20.25" thickTop="1" x14ac:dyDescent="0.5">
@@ -1010,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,253 +1051,316 @@
         <v>4</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>2</v>
+        <v>46</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>0</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>2</v>
+        <v>47</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>2</v>
+        <v>49</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>2</v>
+        <v>50</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>44</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="20"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>44</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="20"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>44</v>
-      </c>
+      <c r="A11" s="4"/>
+      <c r="B11" s="20"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>44</v>
+      <c r="B31" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1294,7 +1376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1312,18 +1394,18 @@
         <v>4</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1354,10 +1436,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1389,10 +1471,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -1427,10 +1509,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>